<commit_message>
fixing documentation parsing and rendering issues, handling for descriptions missing from schema and wiki
</commit_message>
<xml_diff>
--- a/excel/ODM.xlsx
+++ b/excel/ODM.xlsx
@@ -14,7 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MetaDataVersion" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DocumentRef" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PDFPageRef" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="leaf" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Leaf" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Include" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standards" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Standard" sheetId="11" state="visible" r:id="rId11"/>
@@ -1214,14 +1214,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TelecomType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ValueRef</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Email,Pager,Phone,Fax,SMS,URL,Other"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3464,7 +3482,7 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>leafRef</t>
+          <t>LeafRef</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
@@ -3911,7 +3929,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -4952,7 +4970,7 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>leafRef</t>
+          <t>LeafRef</t>
         </is>
       </c>
     </row>
@@ -5408,7 +5426,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>leafID</t>
+          <t>LeafID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5537,7 +5555,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Level</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -5755,7 +5773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5776,36 +5794,46 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Level</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>DescriptionRef</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>StudyTargetPopulationRefRef</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>StudyInterventionRefRef</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>StudyEndPointRefRef</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>IntercurrentEventRef</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>SummaryMeasureRef</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Primary,Secondary,Exploratory"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6183,7 +6211,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Title</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated URLs for release, simpler index page diagram
</commit_message>
<xml_diff>
--- a/excel/ODM.xlsx
+++ b/excel/ODM.xlsx
@@ -639,7 +639,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1458,7 +1458,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -1484,7 +1484,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2150,7 +2150,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -3775,7 +3775,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_language</t>
+          <t>language</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -4285,7 +4285,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -4985,7 +4985,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -6573,7 +6573,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>
@@ -6845,7 +6845,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>_content</t>
+          <t>content</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
prettier camelCase slot names
</commit_message>
<xml_diff>
--- a/excel/ODM.xlsx
+++ b/excel/ODM.xlsx
@@ -572,12 +572,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ContextRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
         </is>
       </c>
     </row>
@@ -603,12 +603,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -795,7 +795,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ImageFileName</t>
+          <t>imageFileName</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>MimeType</t>
+          <t>mimeType</t>
         </is>
       </c>
     </row>
@@ -831,47 +831,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Role</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>role</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>LocationOID</t>
+          <t>locationOID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>PartOfOrganizationOID</t>
+          <t>partOfOrganizationOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AddressRef</t>
+          <t>address</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>TelecomRef</t>
+          <t>telecom</t>
         </is>
       </c>
     </row>
@@ -902,47 +902,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Role</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>role</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>OrganizationOID</t>
+          <t>organizationOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MetaDataVersionRefRef</t>
+          <t>metaDataVersionRef</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AddressRef</t>
+          <t>address</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>TelecomRef</t>
+          <t>telecom</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
     </row>
@@ -968,42 +968,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StreetNameRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>HouseNumberRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CityRef</t>
+          <t>streetName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>houseNumber</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>city</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>StateProvRef</t>
+          <t>stateProv</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CountryRef</t>
+          <t>country</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>PostalCodeRef</t>
+          <t>postalCode</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>GeoPositionRef</t>
+          <t>geoPosition</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>OtherTextRef</t>
+          <t>otherText</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StandardRef</t>
+          <t>standard</t>
         </is>
       </c>
     </row>
@@ -1055,12 +1055,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TelecomType</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ValueRef</t>
+          <t>telecomType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
         </is>
       </c>
     </row>
@@ -1247,17 +1247,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Longitude</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Latitude</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Altitude</t>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>altitude</t>
         </is>
       </c>
     </row>
@@ -1309,17 +1309,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>EffectiveDate</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>effectiveDate</t>
         </is>
       </c>
     </row>
@@ -1345,37 +1345,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Type</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>PublishingSet</t>
+          <t>publishingSet</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Version</t>
+          <t>version</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>status</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
     </row>
@@ -1412,22 +1412,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Methodology</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>MeaningRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>methodology</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>meaning</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LegalReasonRef</t>
+          <t>legalReason</t>
         </is>
       </c>
     </row>
@@ -1510,32 +1510,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ItemGroupDataRef</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>itemGroupData</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1561,42 +1561,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>SubjectDataRef</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>subjectData</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ItemGroupDataRef</t>
+          <t>itemGroupData</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1622,47 +1622,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SubjectKey</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>TransactionTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>InvestigatorRefRef</t>
+          <t>subjectKey</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>transactionType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>investigatorRef</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SiteRefRef</t>
+          <t>siteRef</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StudyEventDataRef</t>
+          <t>studyEventData</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>LocationOID</t>
+          <t>locationOID</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>UserOID</t>
+          <t>userOID</t>
         </is>
       </c>
     </row>
@@ -1745,42 +1745,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEventOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>StudyEventRepeatKey</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>TransactionTypeRef</t>
+          <t>studyEventOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>studyEventRepeatKey</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>transactionType</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ItemGroupDataRef</t>
+          <t>itemGroupData</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1811,52 +1811,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ItemGroupOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ItemGroupRepeatKey</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>TransactionTypeRef</t>
+          <t>itemGroupOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>itemGroupRepeatKey</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>transactionType</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ItemGroupDataSeq</t>
+          <t>itemGroupDataSeq</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>ItemGroupDataRef</t>
+          <t>itemGroupData</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ItemDataRef</t>
+          <t>itemData</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DocumentRefRef</t>
+          <t>documentRef</t>
         </is>
       </c>
     </row>
@@ -1913,42 +1913,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ItemOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>TransactionTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>IsNull</t>
+          <t>itemOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>transactionType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isNull</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ValueRef</t>
+          <t>value</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>QueryRef</t>
+          <t>query</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signature</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -1982,37 +1982,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>EditPoint</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>UsedMethod</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>UserRefRef</t>
+          <t>editPoint</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>usedMethod</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>userRef</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LocationRefRef</t>
+          <t>locationRef</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DateTimeStampRef</t>
+          <t>dateTimeStamp</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>ReasonForChangeRef</t>
+          <t>reasonForChange</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SourceIDRef</t>
+          <t>sourceID</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>UserOID</t>
+          <t>userOID</t>
         </is>
       </c>
     </row>
@@ -2072,7 +2072,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>LocationOID</t>
+          <t>locationOID</t>
         </is>
       </c>
     </row>
@@ -2176,27 +2176,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>UserRefRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>LocationRefRef</t>
+          <t>iD</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>userRef</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>locationRef</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SignatureRefRef</t>
+          <t>signatureRef</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DateTimeStampRef</t>
+          <t>dateTimeStamp</t>
         </is>
       </c>
     </row>
@@ -2222,7 +2222,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SignatureOID</t>
+          <t>signatureOID</t>
         </is>
       </c>
     </row>
@@ -2248,22 +2248,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>KeySetRef</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>keySet</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>AnnotationRef</t>
+          <t>annotation</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DocumentRefRef</t>
+          <t>documentRef</t>
         </is>
       </c>
     </row>
@@ -2315,42 +2315,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>SubjectKey</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subjectKey</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>StudyEventOID</t>
+          <t>studyEventOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StudyEventRepeatKey</t>
+          <t>studyEventRepeatKey</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>ItemGroupOID</t>
+          <t>itemGroupOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ItemGroupRepeatKey</t>
+          <t>itemGroupRepeatKey</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ItemOID</t>
+          <t>itemOID</t>
         </is>
       </c>
     </row>
@@ -2376,32 +2376,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SeqNum</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>TransactionTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ID</t>
+          <t>seqNum</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>transactionType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>iD</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CommentRef</t>
+          <t>comment</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>FlagRef</t>
+          <t>flag</t>
         </is>
       </c>
     </row>
@@ -2432,12 +2432,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SponsorOrSite</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>TranslatedTextRef</t>
+          <t>sponsorOrSite</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -2468,12 +2468,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>FlagValueRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>FlagTypeRef</t>
+          <t>flagValue</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>flagType</t>
         </is>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CodeListOID</t>
+          <t>codeListOID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2530,7 +2530,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CodeListOID</t>
+          <t>codeListOID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2561,27 +2561,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CodeRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>SystemName</t>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>system</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>systemName</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SystemVersion</t>
+          <t>systemVersion</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Label</t>
+          <t>label</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
     </row>
@@ -2622,47 +2622,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Source</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Target</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>target</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>State</t>
+          <t>state</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>LastUpdateDatetime</t>
+          <t>lastUpdateDatetime</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ValueRef</t>
+          <t>value</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>AuditRecordRef</t>
+          <t>auditRecord</t>
         </is>
       </c>
     </row>
@@ -2699,7 +2699,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SeqNum</t>
+          <t>seqNum</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2730,87 +2730,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>FileTypeRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>GranularityRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ContextRef</t>
+          <t>fileType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>granularity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>context</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>FileOID</t>
+          <t>fileOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CreationDateTime</t>
+          <t>creationDateTime</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>PriorFileOID</t>
+          <t>priorFileOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AsOfDateTime</t>
+          <t>asOfDateTime</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ODMVersionRef</t>
+          <t>oDMVersion</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Originator</t>
+          <t>originator</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>SourceSystem</t>
+          <t>sourceSystem</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>SourceSystemVersion</t>
+          <t>sourceSystemVersion</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>StudyRef</t>
+          <t>study</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>AdminDataRef</t>
+          <t>adminData</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>ReferenceDataRef</t>
+          <t>referenceData</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>ClinicalDataRef</t>
+          <t>clinicalData</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>AssociationRef</t>
+          <t>association</t>
         </is>
       </c>
     </row>
@@ -2847,17 +2847,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ItemRefRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>itemRef</t>
         </is>
       </c>
     </row>
@@ -2883,7 +2883,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>WhereClauseOID</t>
+          <t>whereClauseOID</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CommentOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>RangeCheckRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>commentOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>rangeCheck</t>
         </is>
       </c>
     </row>
@@ -2945,27 +2945,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEventGroupOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>OrderNumber</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Mandatory</t>
+          <t>studyEventGroupOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orderNumber</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mandatory</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CollectionExceptionConditionOID</t>
+          <t>collectionExceptionConditionOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -2996,52 +2996,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ArmOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>armOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>EpochOID</t>
+          <t>epochOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>StudyEventGroupRefRef</t>
+          <t>studyEventGroupRef</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>StudyEventRefRef</t>
+          <t>studyEventRef</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -3093,22 +3093,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEventOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>OrderNumber</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Mandatory</t>
+          <t>studyEventOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orderNumber</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mandatory</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CollectionExceptionConditionOID</t>
+          <t>collectionExceptionConditionOID</t>
         </is>
       </c>
     </row>
@@ -3139,57 +3139,57 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Repeating</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repeating</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>category</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ItemGroupRefRef</t>
+          <t>itemGroupRef</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -3223,27 +3223,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ItemGroupOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>MethodOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderNumber</t>
+          <t>itemGroupOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>methodOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>orderNumber</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Mandatory</t>
+          <t>mandatory</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CollectionExceptionConditionOID</t>
+          <t>collectionExceptionConditionOID</t>
         </is>
       </c>
     </row>
@@ -3274,122 +3274,122 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Repeating</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repeating</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RepeatingLimit</t>
+          <t>repeatingLimit</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>IsReferenceData</t>
+          <t>isReferenceData</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Structure</t>
+          <t>structure</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ArchiveLocationID</t>
+          <t>archiveLocationID</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>DatasetName</t>
+          <t>datasetName</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Domain</t>
+          <t>domain</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Purpose</t>
+          <t>purpose</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>StandardOID</t>
+          <t>standardOID</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>IsNonStandard</t>
+          <t>isNonStandard</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>HasNoData</t>
+          <t>hasNoData</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>ClassRef</t>
+          <t>classRef</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>OriginRef</t>
+          <t>origin</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>LeafRef</t>
+          <t>leaf</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>ItemGroupRefRef</t>
+          <t>itemGroupRef</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>ItemRefRef</t>
+          <t>itemRef</t>
         </is>
       </c>
     </row>
@@ -3429,12 +3429,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>SubClassRef</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>subClass</t>
         </is>
       </c>
     </row>
@@ -3465,12 +3465,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ParentClass</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>parentClass</t>
         </is>
       </c>
     </row>
@@ -3501,87 +3501,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ItemOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>KeySequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>IsNonStandard</t>
+          <t>itemOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>keySequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isNonStandard</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>HasNoData</t>
+          <t>hasNoData</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>MethodOID</t>
+          <t>methodOID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>UnitsItemOID</t>
+          <t>unitsItemOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Repeat</t>
+          <t>repeat</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>other</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Role</t>
+          <t>role</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>RoleCodeListOID</t>
+          <t>roleCodeListOID</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>core</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>PreSpecifiedValue</t>
+          <t>preSpecifiedValue</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>OrderNumber</t>
+          <t>orderNumber</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Mandatory</t>
+          <t>mandatory</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>CollectionExceptionConditionOID</t>
+          <t>collectionExceptionConditionOID</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>OriginRef</t>
+          <t>origin</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>WhereClauseRefRef</t>
+          <t>whereClauseRef</t>
         </is>
       </c>
     </row>
@@ -3624,32 +3624,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Source</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SourceItemsRef</t>
+          <t>sourceItems</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>DocumentRefRef</t>
+          <t>documentRef</t>
         </is>
       </c>
     </row>
@@ -3683,12 +3683,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>SourceItemRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CodingRef</t>
+          <t>sourceItem</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -3714,22 +3714,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ItemOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ItemGroupOID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>MetaDataVersionOID</t>
+          <t>itemOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>itemGroupOID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>metaDataVersionOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
+          <t>studyOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -3739,17 +3739,17 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ResourceRef</t>
+          <t>resource</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -3811,27 +3811,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Attribute</t>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>attribute</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Label</t>
+          <t>label</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>SelectionRef</t>
+          <t>selection</t>
         </is>
       </c>
     </row>
@@ -3857,7 +3857,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Path</t>
+          <t>path</t>
         </is>
       </c>
     </row>
@@ -3883,97 +3883,97 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DataTypeRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dataType</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Length</t>
+          <t>length</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DisplayFormat</t>
+          <t>displayFormat</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>VariableSet</t>
+          <t>variableSet</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>DefinitionRef</t>
+          <t>definition</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>QuestionRef</t>
+          <t>question</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>PromptRef</t>
+          <t>prompt</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>CRFCompletionInstructionsRef</t>
+          <t>cRFCompletionInstructions</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>ImplementationNotesRef</t>
+          <t>implementationNotes</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>CDISCNotesRef</t>
+          <t>cDISCNotes</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>RangeCheckRef</t>
+          <t>rangeCheck</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>CodeListRefRef</t>
+          <t>codeListRef</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>ValueListRefRef</t>
+          <t>valueListRef</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -4004,7 +4004,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4030,7 +4030,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4056,7 +4056,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4082,7 +4082,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4108,7 +4108,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4134,7 +4134,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4160,37 +4160,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ComparatorRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>SoftHard</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ItemOID</t>
+          <t>comparator</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>softHard</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>itemOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ErrorMessageRef</t>
+          <t>errorMessage</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>MethodSignatureRef</t>
+          <t>methodSignature</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>FormalExpressionRef</t>
+          <t>formalExpression</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>CheckValueRef</t>
+          <t>checkValue</t>
         </is>
       </c>
     </row>
@@ -4224,42 +4224,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>StudyName</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ProtocolName</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>studyName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>protocolName</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>VersionID</t>
+          <t>versionID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>VersionName</t>
+          <t>versionName</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>status</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>MetaDataVersionRefRef</t>
+          <t>metaDataVersion</t>
         </is>
       </c>
     </row>
@@ -4311,7 +4311,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4337,7 +4337,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CodeListOID</t>
+          <t>codeListOID</t>
         </is>
       </c>
     </row>
@@ -4363,7 +4363,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ValueListOID</t>
+          <t>valueListOID</t>
         </is>
       </c>
     </row>
@@ -4389,52 +4389,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DataTypeRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dataType</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StandardOID</t>
+          <t>standardOID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>IsNonStandard</t>
+          <t>isNonStandard</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>CodeListItemRef</t>
+          <t>codeListItem</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -4468,52 +4468,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CodedValue</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Rank</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Other</t>
+          <t>codedValue</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>other</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>OrderNumber</t>
+          <t>orderNumber</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ExtendedValue</t>
+          <t>extendedValue</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>DecodeRef</t>
+          <t>decode</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -4547,7 +4547,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TranslatedTextRef</t>
+          <t>translatedText</t>
         </is>
       </c>
     </row>
@@ -4573,47 +4573,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Type</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CommentOID</t>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>MethodSignatureRef</t>
+          <t>methodSignature</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>FormalExpressionRef</t>
+          <t>formalExpression</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>DocumentRefRef</t>
+          <t>documentRef</t>
         </is>
       </c>
     </row>
@@ -4644,12 +4644,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ParameterRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ReturnValueRef</t>
+          <t>parameter</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>returnValue</t>
         </is>
       </c>
     </row>
@@ -4675,22 +4675,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DataTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DefinitionRef</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dataType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>definition</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>OrderNumber</t>
+          <t>orderNumber</t>
         </is>
       </c>
     </row>
@@ -4721,107 +4721,107 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CommentOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>IncludeRef</t>
+          <t>include</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>StandardsRef</t>
+          <t>standards</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AnnotatedCRFRef</t>
+          <t>annotatedCRF</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>SupplementalDocRef</t>
+          <t>supplementalDoc</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>ValueListDefRef</t>
+          <t>valueListDef</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>WhereClauseDefRef</t>
+          <t>whereClauseDef</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ProtocolRef</t>
+          <t>protocol</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>WorkflowDefRef</t>
+          <t>workflowDef</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>StudyEventGroupDefRef</t>
+          <t>studyEventGroupDef</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>StudyEventDefRef</t>
+          <t>studyEventDef</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>ItemGroupDefRef</t>
+          <t>itemGroupDef</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>ItemDefRef</t>
+          <t>itemDef</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>CodeListRefRef</t>
+          <t>codeList</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>ConditionDefRef</t>
+          <t>conditionDef</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>MethodDefRef</t>
+          <t>methodDef</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>CommentDefRef</t>
+          <t>commentDef</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>LeafRef</t>
+          <t>leaf</t>
         </is>
       </c>
     </row>
@@ -4847,22 +4847,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DataTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DefinitionRef</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>dataType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>definition</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>OrderNumber</t>
+          <t>orderNumber</t>
         </is>
       </c>
     </row>
@@ -4893,37 +4893,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CommentOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>commentOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>MethodSignatureRef</t>
+          <t>methodSignature</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>FormalExpressionRef</t>
+          <t>formalExpression</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -4949,17 +4949,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ContextRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CodeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ExternalCodeLibRef</t>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>externalCodeLib</t>
         </is>
       </c>
     </row>
@@ -5011,17 +5011,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Library</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Method</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Version</t>
+          <t>library</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>version</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -5057,17 +5057,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DocumentRefRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>documentRef</t>
         </is>
       </c>
     </row>
@@ -5093,77 +5093,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>StudySummaryRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>StudyStructureRef</t>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>studySummary</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>studyStructure</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>TrialPhaseRef</t>
+          <t>trialPhase</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StudyTimingsRef</t>
+          <t>studyTimings</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>StudyIndicationsRef</t>
+          <t>studyIndications</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>StudyInterventionsRef</t>
+          <t>studyInterventions</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>StudyObjectivesRef</t>
+          <t>studyObjectives</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>StudyEndPointsRef</t>
+          <t>studyEndPoints</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>StudyTargetPopulationRefRef</t>
+          <t>studyTargetPopulation</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>StudyEstimandsRef</t>
+          <t>studyEstimands</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>InclusionExclusionCriteriaRef</t>
+          <t>inclusionExclusionCriteria</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>StudyEventGroupRefRef</t>
+          <t>studyEventGroupRef</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>AliasRef</t>
+          <t>alias</t>
         </is>
       </c>
     </row>
@@ -5189,22 +5189,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ArmRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>EpochRef</t>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>arm</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>epoch</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
     </row>
@@ -5230,12 +5230,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ValueRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -5261,7 +5261,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyIndicationRef</t>
+          <t>studyIndication</t>
         </is>
       </c>
     </row>
@@ -5287,12 +5287,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>LeafID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>PDFPageRefRef</t>
+          <t>leafID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>pDFPageRef</t>
         </is>
       </c>
     </row>
@@ -5318,17 +5318,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CodingRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5354,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyInterventionRefRef</t>
+          <t>studyIntervention</t>
         </is>
       </c>
     </row>
@@ -5380,17 +5380,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CodingRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -5416,7 +5416,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyObjectiveRef</t>
+          <t>studyObjective</t>
         </is>
       </c>
     </row>
@@ -5442,27 +5442,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Level</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StudyEndPointRefRef</t>
+          <t>studyEndPointRef</t>
         </is>
       </c>
     </row>
@@ -5493,12 +5493,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEndPointOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>OrderNumber</t>
+          <t>studyEndPointOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orderNumber</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEndPointRefRef</t>
+          <t>studyEndPoint</t>
         </is>
       </c>
     </row>
@@ -5550,32 +5550,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Type</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Level</t>
+          <t>level</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>FormalExpressionRef</t>
+          <t>formalExpression</t>
         </is>
       </c>
     </row>
@@ -5609,27 +5609,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>FormalExpressionRef</t>
+          <t>formalExpression</t>
         </is>
       </c>
     </row>
@@ -5655,7 +5655,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyEstimandRef</t>
+          <t>studyEstimand</t>
         </is>
       </c>
     </row>
@@ -5681,27 +5681,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>PageRefs</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>FirstPage</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>LastPage</t>
+          <t>pageRefs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>firstPage</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>lastPage</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>TitleRef</t>
+          <t>title</t>
         </is>
       </c>
     </row>
@@ -5732,47 +5732,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Level</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>level</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StudyTargetPopulationRefRef</t>
+          <t>studyTargetPopulationRef</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>StudyInterventionRefRef</t>
+          <t>studyInterventionRef</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>StudyEndPointRefRef</t>
+          <t>studyEndPointRef</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>IntercurrentEventRef</t>
+          <t>intercurrentEvent</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>SummaryMeasureRef</t>
+          <t>summaryMeasure</t>
         </is>
       </c>
     </row>
@@ -5803,12 +5803,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>InclusionCriteriaRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ExclusionCriteriaRef</t>
+          <t>inclusionCriteria</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>exclusionCriteria</t>
         </is>
       </c>
     </row>
@@ -5834,7 +5834,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CriterionRef</t>
+          <t>criterion</t>
         </is>
       </c>
     </row>
@@ -5860,7 +5860,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>CriterionRef</t>
+          <t>criterion</t>
         </is>
       </c>
     </row>
@@ -5886,7 +5886,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyTargetPopulationOID</t>
+          <t>studyTargetPopulationOID</t>
         </is>
       </c>
     </row>
@@ -5912,7 +5912,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyInterventionOID</t>
+          <t>studyInterventionOID</t>
         </is>
       </c>
     </row>
@@ -5938,7 +5938,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -5964,7 +5964,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -5990,22 +5990,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>WorkflowRefRef</t>
+          <t>workflowRef</t>
         </is>
       </c>
     </row>
@@ -6031,22 +6031,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>SequenceNumber</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequenceNumber</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -6072,7 +6072,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>iD</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>TitleRef</t>
+          <t>title</t>
         </is>
       </c>
     </row>
@@ -6108,7 +6108,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>WorkflowOID</t>
+          <t>workflowOID</t>
         </is>
       </c>
     </row>
@@ -6134,7 +6134,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyParameterRef</t>
+          <t>studyParameter</t>
         </is>
       </c>
     </row>
@@ -6160,27 +6160,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Term</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ShortName</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>shortName</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>ParameterValueRef</t>
+          <t>parameterValue</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -6206,12 +6206,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ValueRef</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CodingRef</t>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -6237,7 +6237,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyTimingRef</t>
+          <t>studyTiming</t>
         </is>
       </c>
     </row>
@@ -6263,32 +6263,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>AbsoluteTimingConstraintRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>absoluteTimingConstraint</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RelativeTimingConstraintRef</t>
+          <t>relativeTimingConstraint</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>TransitionTimingConstraintRef</t>
+          <t>transitionTimingConstraint</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>DurationTimingConstraintRef</t>
+          <t>durationTimingConstraint</t>
         </is>
       </c>
     </row>
@@ -6314,47 +6314,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>TransitionOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>transitionOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>MethodOID</t>
+          <t>methodOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>TimepointTarget</t>
+          <t>timepointTarget</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>TimepointPreWindow</t>
+          <t>timepointPreWindow</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>TimepointPostWindow</t>
+          <t>timepointPostWindow</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -6385,42 +6385,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>StudyEventGroupOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>studyEventGroupOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>StudyEventOID</t>
+          <t>studyEventOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>TimepointTarget</t>
+          <t>timepointTarget</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>TimepointPreWindow</t>
+          <t>timepointPreWindow</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>TimepointPostWindow</t>
+          <t>timepointPostWindow</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -6446,47 +6446,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>PredecessorOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>predecessorOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SuccessorOID</t>
+          <t>successorOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>TimepointRelativeTarget</t>
+          <t>timepointRelativeTarget</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>TimepointPreWindow</t>
+          <t>timepointPreWindow</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>TimepointPostWindow</t>
+          <t>timepointPostWindow</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -6517,37 +6517,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>StructuralElementOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>structuralElementOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DurationTarget</t>
+          <t>durationTarget</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DurationPreWindow</t>
+          <t>durationPreWindow</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>DurationPostWindow</t>
+          <t>durationPostWindow</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
     </row>
@@ -6599,37 +6599,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DescriptionRef</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>WorkflowStartRef</t>
+          <t>workflowStart</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>WorkflowEndRef</t>
+          <t>workflowEnd</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>TransitionRef</t>
+          <t>transition</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>BranchingRef</t>
+          <t>branching</t>
         </is>
       </c>
     </row>
@@ -6655,7 +6655,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StartOID</t>
+          <t>startOID</t>
         </is>
       </c>
     </row>
@@ -6681,32 +6681,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>SourceOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sourceOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>TargetOID</t>
+          <t>targetOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>StartConditionOID</t>
+          <t>startConditionOID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>EndConditionOID</t>
+          <t>endConditionOID</t>
         </is>
       </c>
     </row>
@@ -6732,27 +6732,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Type</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>TargetTransitionRef</t>
+          <t>targetTransition</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>DefaultTransitionRef</t>
+          <t>defaultTransition</t>
         </is>
       </c>
     </row>
@@ -6783,12 +6783,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TargetTransitionOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ConditionOID</t>
+          <t>targetTransitionOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>conditionOID</t>
         </is>
       </c>
     </row>
@@ -6814,7 +6814,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TargetTransitionOID</t>
+          <t>targetTransitionOID</t>
         </is>
       </c>
     </row>
@@ -6840,7 +6840,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>EndOID</t>
+          <t>endOID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6871,27 +6871,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ConditionOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>conditionOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>DescriptionRef</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>CodingRef</t>
+          <t>coding</t>
         </is>
       </c>
     </row>
@@ -6917,27 +6917,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>StudyOID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>UserRefRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrganizationRef</t>
+          <t>studyOID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>organization</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LocationRefRef</t>
+          <t>location</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>SignatureDefRef</t>
+          <t>signatureDef</t>
         </is>
       </c>
     </row>
@@ -6963,67 +6963,67 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>OID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>UserTypeRef</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrganizationOID</t>
+          <t>oID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>userType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>organizationOID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>LocationOID</t>
+          <t>locationOID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>UserNameRef</t>
+          <t>userName</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>PrefixRef</t>
+          <t>prefix</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SuffixRef</t>
+          <t>suffix</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>FullNameRef</t>
+          <t>fullName</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>GivenNameRef</t>
+          <t>givenName</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>FamilyNameRef</t>
+          <t>familyName</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ImageRef</t>
+          <t>image</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>AddressRef</t>
+          <t>address</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>TelecomRef</t>
+          <t>telecom</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved references by detecting targets for oidref type slots
</commit_message>
<xml_diff>
--- a/excel/ODM.xlsx
+++ b/excel/ODM.xlsx
@@ -831,7 +831,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -902,7 +902,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1345,7 +1345,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1412,7 +1412,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>iD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>iD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -2622,7 +2622,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2847,7 +2847,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2909,7 +2909,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2996,7 +2996,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -3139,7 +3139,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -3274,7 +3274,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>classRef</t>
+          <t>itemGroupClass</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -3883,7 +3883,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -4224,7 +4224,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -4389,7 +4389,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -4573,7 +4573,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -4721,7 +4721,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -4893,7 +4893,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5057,7 +5057,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5318,7 +5318,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5442,7 +5442,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5550,7 +5550,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5609,7 +5609,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5732,7 +5732,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5990,7 +5990,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6031,7 +6031,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6072,7 +6072,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>iD</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6160,7 +6160,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6263,7 +6263,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6314,7 +6314,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6385,7 +6385,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6446,7 +6446,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6517,7 +6517,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6599,7 +6599,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6681,7 +6681,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6732,7 +6732,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6871,7 +6871,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6963,7 +6963,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>oID</t>
+          <t>OID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">

</xml_diff>